<commit_message>
model with minimize function
</commit_message>
<xml_diff>
--- a/Analysis/Data/CheckEqs.xlsx
+++ b/Analysis/Data/CheckEqs.xlsx
@@ -607,12 +607,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -658,6 +652,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -786,11 +786,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="161066368"/>
-        <c:axId val="161076736"/>
+        <c:axId val="157024640"/>
+        <c:axId val="157026560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="161066368"/>
+        <c:axId val="157024640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -814,19 +814,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="161076736"/>
+        <c:crossAx val="157026560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="161076736"/>
+        <c:axId val="157026560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -850,21 +849,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="161066368"/>
+        <c:crossAx val="157024640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1476,11 +1473,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="161205248"/>
-        <c:axId val="162088064"/>
+        <c:axId val="157458432"/>
+        <c:axId val="157460352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="161205248"/>
+        <c:axId val="157458432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1493,12 +1490,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="162088064"/>
+        <c:crossAx val="157460352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="162088064"/>
+        <c:axId val="157460352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1512,7 +1509,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="161205248"/>
+        <c:crossAx val="157458432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2130,11 +2127,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="169626240"/>
-        <c:axId val="169628416"/>
+        <c:axId val="159227264"/>
+        <c:axId val="159233536"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="169626240"/>
+        <c:axId val="159227264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2147,12 +2144,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169628416"/>
+        <c:crossAx val="159233536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="169628416"/>
+        <c:axId val="159233536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2166,7 +2163,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169626240"/>
+        <c:crossAx val="159227264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2784,11 +2781,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="170328064"/>
-        <c:axId val="170329984"/>
+        <c:axId val="159341568"/>
+        <c:axId val="159356032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="170328064"/>
+        <c:axId val="159341568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2801,12 +2798,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170329984"/>
+        <c:crossAx val="159356032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="170329984"/>
+        <c:axId val="159356032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2820,7 +2817,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170328064"/>
+        <c:crossAx val="159341568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2856,7 +2853,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3439,30 +3435,29 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="160445952"/>
-        <c:axId val="160447872"/>
+        <c:axId val="162969856"/>
+        <c:axId val="162976128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="160445952"/>
+        <c:axId val="162969856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="160447872"/>
+        <c:crossAx val="162976128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="160447872"/>
+        <c:axId val="162976128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3470,21 +3465,19 @@
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="160445952"/>
+        <c:crossAx val="162969856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4147,11 +4140,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="170172416"/>
-        <c:axId val="170173952"/>
+        <c:axId val="169051264"/>
+        <c:axId val="169052800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="170172416"/>
+        <c:axId val="169051264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4161,12 +4154,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170173952"/>
+        <c:crossAx val="169052800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="170173952"/>
+        <c:axId val="169052800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4177,14 +4170,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170172416"/>
+        <c:crossAx val="169051264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -14389,25 +14381,25 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
       <c r="E5" s="4"/>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="J5" s="7" t="s">
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="J5" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7" t="s">
+      <c r="K5" s="24"/>
+      <c r="L5" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="M5" s="7"/>
+      <c r="M5" s="24"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -19487,25 +19479,25 @@
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
       <c r="E5" s="4"/>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="J5" s="7" t="s">
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="J5" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7" t="s">
+      <c r="K5" s="24"/>
+      <c r="L5" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="M5" s="7"/>
+      <c r="M5" s="24"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -25581,42 +25573,42 @@
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="J5" s="8" t="s">
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="J5" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="25"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
       <c r="E6" s="4"/>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="J6" s="7" t="s">
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="J6" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7" t="s">
+      <c r="K6" s="24"/>
+      <c r="L6" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="M6" s="7"/>
+      <c r="M6" s="24"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -31310,42 +31302,42 @@
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="K5" s="8" t="s">
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="K5" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="25"/>
+      <c r="N5" s="25"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
       <c r="E6" s="4"/>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="K6" s="7" t="s">
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="K6" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7" t="s">
+      <c r="L6" s="24"/>
+      <c r="M6" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="N6" s="7"/>
+      <c r="N6" s="24"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -37257,8 +37249,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37269,28 +37261,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="J1" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="19" t="s">
+      <c r="K1" s="17" t="s">
         <v>71</v>
       </c>
     </row>
@@ -37298,101 +37290,101 @@
       <c r="C2" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="14">
+      <c r="D2" s="12">
         <v>0.2</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="13">
         <f>274.15+20</f>
         <v>294.14999999999998</v>
       </c>
-      <c r="F2" s="14">
+      <c r="F2" s="12">
         <v>0.4</v>
       </c>
-      <c r="G2" s="15">
-        <f t="shared" ref="G2:K2" si="0">274.15+20</f>
+      <c r="G2" s="13">
+        <f t="shared" ref="G2" si="0">274.15+20</f>
         <v>294.14999999999998</v>
       </c>
-      <c r="H2" s="14">
+      <c r="H2" s="12">
         <v>0.2</v>
       </c>
-      <c r="I2" s="15">
+      <c r="I2" s="13">
         <f>274.15+30</f>
         <v>304.14999999999998</v>
       </c>
-      <c r="J2" s="14">
+      <c r="J2" s="12">
         <v>0.4</v>
       </c>
-      <c r="K2" s="15">
+      <c r="K2" s="13">
         <f>274.15+30</f>
         <v>304.14999999999998</v>
       </c>
     </row>
     <row r="3" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="10" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="4" spans="3:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="J4" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="K4" s="9" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="5" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="8">
         <v>30</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="8">
         <v>2.3300000000000001E-2</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="8">
         <v>41</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="8">
         <v>1.7100000000000001E-2</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H5" s="8">
         <v>28</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="8">
         <v>2.4799999999999999E-2</v>
       </c>
-      <c r="J5" s="10">
+      <c r="J5" s="8">
         <v>30</v>
       </c>
-      <c r="K5" s="10">
+      <c r="K5" s="8">
         <v>2.2700000000000001E-2</v>
       </c>
     </row>
@@ -37427,7 +37419,7 @@
         <v>40.981207702631863</v>
       </c>
       <c r="G9" s="6"/>
-      <c r="H9" s="24">
+      <c r="H9" s="22">
         <f>$D$9*H20*$H$25</f>
         <v>21.752915336928535</v>
       </c>
@@ -37451,7 +37443,7 @@
         <v>33.819373146171706</v>
       </c>
       <c r="G10" s="6"/>
-      <c r="H10" s="24">
+      <c r="H10" s="22">
         <f>$D$9*H21*$H$25</f>
         <v>14.388201068038928</v>
       </c>
@@ -37548,7 +37540,7 @@
       <c r="C19" t="s">
         <v>63</v>
       </c>
-      <c r="D19" s="25" t="s">
+      <c r="D19" s="23" t="s">
         <v>66</v>
       </c>
       <c r="E19" s="6"/>
@@ -37634,7 +37626,7 @@
       <c r="C24" t="s">
         <v>63</v>
       </c>
-      <c r="D24" s="25" t="s">
+      <c r="D24" s="23" t="s">
         <v>65</v>
       </c>
       <c r="E24" s="6"/>
@@ -37658,7 +37650,7 @@
         <v>1</v>
       </c>
       <c r="G25" s="6"/>
-      <c r="H25" s="24">
+      <c r="H25" s="22">
         <f>EXP($E$40*(1/I2 - 1/$E$2))</f>
         <v>0.72509717789761785</v>
       </c>
@@ -37685,18 +37677,18 @@
       </c>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A35" s="20" t="s">
+      <c r="A35" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="B35" s="21" t="s">
+      <c r="B35" s="19" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A36" s="22" t="s">
+      <c r="A36" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="B36" s="21">
+      <c r="B36" s="19">
         <v>0.45</v>
       </c>
     </row>
@@ -37706,33 +37698,33 @@
       </c>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A39" s="20" t="s">
+      <c r="A39" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="B39" s="21" t="s">
+      <c r="B39" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="C39" s="21" t="s">
+      <c r="C39" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="D39" s="21" t="s">
+      <c r="D39" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="E39" s="23" t="s">
+      <c r="E39" s="21" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A40" s="22" t="s">
+      <c r="A40" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="B40" s="21">
+      <c r="B40" s="19">
         <v>1</v>
       </c>
-      <c r="C40" s="21">
+      <c r="C40" s="19">
         <v>23.91</v>
       </c>
-      <c r="D40" s="21">
+      <c r="D40" s="19">
         <v>8.3140000000000002E-3</v>
       </c>
       <c r="E40" s="6">
@@ -37742,28 +37734,28 @@
     </row>
     <row r="41" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="42" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A42" s="20"/>
-      <c r="B42" s="16" t="s">
+      <c r="A42" s="18"/>
+      <c r="B42" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="C42" s="16" t="s">
+      <c r="C42" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="D42" s="16" t="s">
+      <c r="D42" s="14" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A43" s="22" t="s">
+      <c r="A43" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="B43" s="21">
+      <c r="B43" s="19">
         <v>0.43</v>
       </c>
-      <c r="C43" s="21">
+      <c r="C43" s="19">
         <v>0.19</v>
       </c>
-      <c r="D43" s="21">
+      <c r="D43" s="19">
         <v>0.5</v>
       </c>
     </row>
@@ -37819,10 +37811,10 @@
       <c r="C55" t="s">
         <v>89</v>
       </c>
-      <c r="D55" s="25" t="s">
+      <c r="D55" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="E55" s="25" t="s">
+      <c r="E55" s="23" t="s">
         <v>65</v>
       </c>
       <c r="F55" t="s">

</xml_diff>